<commit_message>
WORKING: multiple tabs Version 2
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheetFiles/BUTTON_AUTOSTAR2.xlsx
+++ b/src/main/resources/spreadsheetFiles/BUTTON_AUTOSTAR2.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t xml:space="preserve">Drives</t>
   </si>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Intranet</t>
   </si>
   <si>
-    <t xml:space="preserve">C:</t>
+    <t xml:space="preserve">GOOGLE</t>
   </si>
   <si>
     <t xml:space="preserve">Github</t>
@@ -49,24 +49,6 @@
     <t xml:space="preserve">Router</t>
   </si>
   <si>
-    <t xml:space="preserve">D:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biocentury</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gapminder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Google Datasearch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kaggle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OurWorldInData</t>
-  </si>
-  <si>
     <t xml:space="preserve">app1</t>
   </si>
   <si>
@@ -79,7 +61,7 @@
     <t xml:space="preserve">intra1</t>
   </si>
   <si>
-    <t xml:space="preserve">C:\</t>
+    <t xml:space="preserve">www.google.de</t>
   </si>
   <si>
     <t xml:space="preserve">www.github.com</t>
@@ -91,24 +73,6 @@
     <t xml:space="preserve">https://192.168.178.1/</t>
   </si>
   <si>
-    <t xml:space="preserve">D:\</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.bio-century.net</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.gapminder.org/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://datasetsearch.research.google.com/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.kaggle.com/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://ourworldindata.org/</t>
-  </si>
-  <si>
     <t xml:space="preserve">246,194,62</t>
   </si>
   <si>
@@ -116,9 +80,6 @@
   </si>
   <si>
     <t xml:space="preserve">250,250,250</t>
-  </si>
-  <si>
-    <t xml:space="preserve">231,74,59</t>
   </si>
 </sst>
 </file>
@@ -129,11 +90,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -154,12 +116,6 @@
       <u val="single"/>
       <sz val="10"/>
       <color rgb="FF0563C1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -237,15 +193,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -346,7 +302,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -383,47 +339,31 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="C4" s="4"/>
       <c r="D4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
-      <c r="C5" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="C5" s="4"/>
       <c r="D5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="C6" s="4"/>
       <c r="D6" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Expasy"/>
-    <hyperlink ref="C3" r:id="rId2" display="Gapminder"/>
-    <hyperlink ref="C4" r:id="rId3" display="Google Datasearch"/>
-    <hyperlink ref="C5" r:id="rId4" display="Kaggle"/>
-    <hyperlink ref="C6" r:id="rId5" display="OurWorldInData"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -443,7 +383,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -464,52 +404,40 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="C4" s="3"/>
       <c r="D4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
   </sheetData>
@@ -531,7 +459,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -558,59 +486,47 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
       <c r="D3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
-      <c r="C4" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="C4" s="6"/>
       <c r="D4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="C5" s="6"/>
       <c r="D5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="6" t="s">
-        <v>27</v>
-      </c>
+      <c r="C6" s="6"/>
       <c r="D6" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="www.github.com"/>
-    <hyperlink ref="D2" r:id="rId2" display="https://192.168.178.1/"/>
-    <hyperlink ref="B3" r:id="rId3" display="www.bio-century.net"/>
+    <hyperlink ref="A2" r:id="rId1" display="www.google.de"/>
+    <hyperlink ref="B2" r:id="rId2" display="www.github.com"/>
+    <hyperlink ref="D2" r:id="rId3" display="https://192.168.178.1/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -630,7 +546,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J27" activeCellId="0" sqref="J27"/>
+      <selection pane="topLeft" activeCell="G47" activeCellId="0" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -651,51 +567,39 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="C4" s="3"/>
       <c r="D4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8"/>
-      <c r="C6" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="C6" s="3"/>
       <c r="D6" s="8"/>
     </row>
   </sheetData>

</xml_diff>